<commit_message>
Agregue telefonos de contacto y estado de planilla de salud
</commit_message>
<xml_diff>
--- a/Listado alumnos.xlsx
+++ b/Listado alumnos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grupo Partener\Mi unidad\TUDAI\PRIMER AÑO\SEGUNDO CUATRIMESTRE\TIO\PRACTICA\TPE- Grupo 19\2. Informe\Sofi y Adri\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grupo Partener\Mi unidad\TUDAI\PRIMER AÑO\SEGUNDO CUATRIMESTRE\TIO\PRACTICA\TPE Git- Grupo 19\Activate-GYM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9840264B-49E9-4894-BC28-3EF982B7AB3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BDF2D8-701F-4EE7-9A57-CAA53B1D61D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D1944C11-2897-435E-8759-E481085A5686}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
   <si>
     <t>Nombre y Apellido</t>
   </si>
@@ -164,9 +164,6 @@
     <t>Arquitecto</t>
   </si>
   <si>
-    <t>Direccion</t>
-  </si>
-  <si>
     <t>Contacto</t>
   </si>
   <si>
@@ -180,6 +177,15 @@
   </si>
   <si>
     <t>Impago</t>
+  </si>
+  <si>
+    <t>Planilla Salud</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -247,11 +253,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,14 +577,14 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -587,389 +595,465 @@
         <v>43</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>46</v>
+      <c r="G1" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="B2" s="1">
+        <v>2494795241</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2">
+      <c r="E2" s="2">
         <v>1800</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>47</v>
+      <c r="F2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="B3" s="1">
+        <v>2494795246</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2">
+      <c r="E3" s="2">
         <v>2700</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>47</v>
+      <c r="F3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="B4" s="1">
+        <v>2494795263</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="2">
+      <c r="E4" s="2">
         <v>1800</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>48</v>
+      <c r="F4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="B5" s="1">
+        <v>2494795208</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="2">
+      <c r="E5" s="2">
         <v>1200</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>47</v>
+      <c r="F5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="B6" s="1">
+        <v>2494536494</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="2">
+      <c r="E6" s="2">
         <v>1800</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>47</v>
+      <c r="F6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="B7" s="1">
+        <v>2494535939</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="2">
+      <c r="E7" s="2">
         <v>2300</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>48</v>
+      <c r="F7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="B8" s="1">
+        <v>2494480384</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="2">
+      <c r="E8" s="2">
         <v>2300</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>47</v>
+      <c r="F8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="B9" s="1">
+        <v>2494485939</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="2">
+      <c r="E9" s="2">
         <v>1800</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>47</v>
+      <c r="F9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="B10" s="1">
+        <v>2494481495</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="2">
+      <c r="E10" s="2">
         <v>1800</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>47</v>
+      <c r="F10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="B11" s="1">
+        <v>2494485939</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="D11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="2">
+      <c r="E11" s="2">
         <v>1800</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>47</v>
+      <c r="F11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="B12" s="1">
+        <v>2494478162</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="D12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="2">
+      <c r="E12" s="2">
         <v>2700</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>48</v>
+      <c r="F12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="B13" s="1">
+        <v>2494556639</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="2">
+      <c r="E13" s="2">
         <v>1800</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>47</v>
+      <c r="F13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="B14" s="1">
+        <v>2494546640</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="D14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="2">
+      <c r="E14" s="2">
         <v>1200</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>47</v>
+      <c r="F14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="B15" s="1">
+        <v>2494624417</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="2">
+      <c r="E15" s="2">
         <v>1800</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>48</v>
+      <c r="F15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="B16" s="1">
+        <v>2494628861</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="2">
+      <c r="E16" s="2">
         <v>2300</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>47</v>
+      <c r="F16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="B17" s="1">
+        <v>2494628806</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="2">
+      <c r="E17" s="2">
         <v>2300</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>47</v>
+      <c r="F17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="B18" s="1">
+        <v>2494370092</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="2">
+      <c r="E18" s="2">
         <v>2700</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>47</v>
+      <c r="F18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="B19" s="1">
+        <v>2494369537</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="2">
+      <c r="E19" s="2">
         <v>1800</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>48</v>
+      <c r="F19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="B20" s="1">
+        <v>2494313982</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="2">
+      <c r="E20" s="2">
         <v>1200</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>48</v>
+      <c r="F20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G20" xr:uid="{9D5A4CB0-260F-47EB-85CF-C5CC3EE00AC0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F20" xr:uid="{9D5A4CB0-260F-47EB-85CF-C5CC3EE00AC0}">
       <formula1>"Pago, Impago"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F20" xr:uid="{71F38E75-20A8-4612-AA33-5F9BF98E9887}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E20" xr:uid="{71F38E75-20A8-4612-AA33-5F9BF98E9887}">
       <formula1>"$1200, $1800, $2300, $2700"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Aplique formato condicional a los que adeudan la cuota y/o la ficha de salud
</commit_message>
<xml_diff>
--- a/Listado alumnos.xlsx
+++ b/Listado alumnos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grupo Partener\Mi unidad\TUDAI\PRIMER AÑO\SEGUNDO CUATRIMESTRE\TIO\PRACTICA\TPE Git- Grupo 19\Activate-GYM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BDF2D8-701F-4EE7-9A57-CAA53B1D61D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F56F99-002F-46C4-AD91-848A13AA32CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D1944C11-2897-435E-8759-E481085A5686}"/>
   </bookViews>
@@ -264,7 +264,99 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -577,7 +669,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,6 +1141,16 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Impago"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"NO"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F20" xr:uid="{9D5A4CB0-260F-47EB-85CF-C5CC3EE00AC0}">
       <formula1>"Pago, Impago"</formula1>

</xml_diff>